<commit_message>
Add language selection on headers
</commit_message>
<xml_diff>
--- a/dashboard/docs/texts.xlsx
+++ b/dashboard/docs/texts.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
   <workbookPr/>
   <sheets>
-    <sheet state="visible" name="general" sheetId="1" r:id="rId3"/>
+    <sheet state="visible" name="General" sheetId="1" r:id="rId3"/>
     <sheet state="visible" name="Login" sheetId="2" r:id="rId4"/>
   </sheets>
   <definedNames/>
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="23">
   <si>
     <t>lang_en</t>
   </si>
@@ -32,25 +32,19 @@
     <t>txtCopyright</t>
   </si>
   <si>
+    <t>Copyright Blockpass ©2018</t>
+  </si>
+  <si>
+    <t>著作権 Blockpass ©2018</t>
+  </si>
+  <si>
     <t>txtLogin</t>
   </si>
   <si>
-    <t>Copyright Blockpass ©2018</t>
-  </si>
-  <si>
     <t>Login</t>
   </si>
   <si>
-    <t>Copyright Blockpass ©2019</t>
-  </si>
-  <si>
-    <t>Copyright Blockpass ©2020</t>
-  </si>
-  <si>
-    <t>Copyright Blockpass ©2021</t>
-  </si>
-  <si>
-    <t>Copyright Blockpass ©2022</t>
+    <t>ログイン</t>
   </si>
   <si>
     <t>txtUsernamePlaceholder</t>
@@ -59,29 +53,41 @@
     <t>username</t>
   </si>
   <si>
+    <t>ユーザー名</t>
+  </si>
+  <si>
     <t>txtInvalidUsername</t>
   </si>
   <si>
     <t>Invalid user name</t>
   </si>
   <si>
+    <t>無効なユーザー名</t>
+  </si>
+  <si>
     <t>txtPasswordPlaceholder</t>
   </si>
   <si>
     <t>password</t>
   </si>
   <si>
+    <t>パスワード</t>
+  </si>
+  <si>
     <t>txtInvalidPassword</t>
   </si>
   <si>
     <t>Invalid password</t>
+  </si>
+  <si>
+    <t>無効なパスワード</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="5">
+  <fonts count="6">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -103,13 +109,23 @@
       <name val="Calibri"/>
     </font>
     <font/>
+    <font>
+      <color rgb="FF212121"/>
+      <name val="Inherit"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="lightGray"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+        <bgColor rgb="FFFFFFFF"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -118,7 +134,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -133,6 +149,9 @@
     </xf>
     <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="2" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
+      <alignment horizontal="left" readingOrder="0" shrinkToFit="0" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -183,19 +202,19 @@
         <v>5</v>
       </c>
       <c r="B2" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="4" t="s">
-        <v>9</v>
-      </c>
       <c r="D2" s="4" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
     </row>
   </sheetData>
@@ -233,62 +252,62 @@
     </row>
     <row r="2">
       <c r="A2" s="4" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="C2" s="4" t="s">
-        <v>8</v>
+        <v>9</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>10</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C3" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="B3" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="C3" s="4" t="s">
-        <v>14</v>
-      </c>
       <c r="D3" s="4" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B4" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="B4" s="4" t="s">
+      <c r="C4" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="C4" s="4" t="s">
-        <v>16</v>
-      </c>
       <c r="D4" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F4" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="5">
@@ -298,8 +317,8 @@
       <c r="B5" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="C5" s="4" t="s">
-        <v>18</v>
+      <c r="C5" s="5" t="s">
+        <v>19</v>
       </c>
       <c r="D5" s="4" t="s">
         <v>18</v>
@@ -313,22 +332,22 @@
     </row>
     <row r="6">
       <c r="A6" s="4" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="C6" s="4" t="s">
-        <v>20</v>
+        <v>21</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>22</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="F6" s="4" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
     </row>
   </sheetData>

</xml_diff>